<commit_message>
Part II Finished: tests written.
</commit_message>
<xml_diff>
--- a/OurClues/ClueLayout_Excel.xlsx
+++ b/OurClues/ClueLayout_Excel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="38">
   <si>
     <t>Closet</t>
   </si>
@@ -112,6 +112,24 @@
   </si>
   <si>
     <t>HR</t>
+  </si>
+  <si>
+    <t>Door Direction Test</t>
+  </si>
+  <si>
+    <t>Adj. List Test inside Room</t>
+  </si>
+  <si>
+    <t>Adj. List Test room exits</t>
+  </si>
+  <si>
+    <t>Adj. List Test beside room entrance</t>
+  </si>
+  <si>
+    <t>Walkway scenarios</t>
+  </si>
+  <si>
+    <t>Test Targets</t>
   </si>
 </sst>
 </file>
@@ -127,7 +145,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,6 +182,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -192,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -210,6 +264,42 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -513,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC23"/>
+  <dimension ref="A1:AC30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD17" sqref="AD17"/>
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,7 +616,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -535,10 +625,10 @@
       <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="17" t="s">
         <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -752,7 +842,7 @@
       <c r="AB3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AC3" s="13" t="s">
         <v>1</v>
       </c>
     </row>
@@ -781,7 +871,7 @@
       <c r="H4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="15" t="s">
         <v>23</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -790,7 +880,7 @@
       <c r="K4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="14" t="s">
         <v>11</v>
       </c>
       <c r="M4" s="2" t="s">
@@ -835,7 +925,7 @@
       <c r="AB4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AC4" s="13" t="s">
         <v>21</v>
       </c>
     </row>
@@ -846,13 +936,13 @@
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="16" t="s">
         <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -864,7 +954,7 @@
       <c r="H5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="16" t="s">
         <v>20</v>
       </c>
       <c r="J5" s="2" t="s">
@@ -918,12 +1008,12 @@
       <c r="AB5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AC5" s="3" t="s">
+      <c r="AC5" s="13" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -932,7 +1022,7 @@
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="17" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -1001,7 +1091,7 @@
       <c r="AB6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AC6" s="3" t="s">
+      <c r="AC6" s="13" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1084,7 +1174,7 @@
       <c r="AB7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AC7" s="3" t="s">
+      <c r="AC7" s="13" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1167,7 +1257,7 @@
       <c r="AB8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AC8" s="3" t="s">
+      <c r="AC8" s="13" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1178,7 +1268,7 @@
       <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -1250,18 +1340,18 @@
       <c r="AB9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AC9" s="3" t="s">
+      <c r="AC9" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="14" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="15" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1276,7 +1366,7 @@
       <c r="G10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="18" t="s">
         <v>20</v>
       </c>
       <c r="I10" s="2" t="s">
@@ -1333,7 +1423,7 @@
       <c r="AB10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AC10" s="3" t="s">
+      <c r="AC10" s="13" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1416,7 +1506,7 @@
       <c r="AB11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AC11" s="3" t="s">
+      <c r="AC11" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1487,7 +1577,7 @@
       <c r="V12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W12" s="2" t="s">
+      <c r="W12" s="17" t="s">
         <v>20</v>
       </c>
       <c r="X12" s="3">
@@ -1499,7 +1589,7 @@
       <c r="AB12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AC12" s="3" t="s">
+      <c r="AC12" s="13" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1579,12 +1669,12 @@
       <c r="AB13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AC13" s="3" t="s">
+      <c r="AC13" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1712,10 +1802,10 @@
       <c r="R15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="S15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="T15" s="6" t="s">
+      <c r="S15" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="T15" s="15" t="s">
         <v>26</v>
       </c>
       <c r="U15" s="1" t="s">
@@ -1753,7 +1843,7 @@
       <c r="G16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I16" s="2" t="s">
@@ -1866,13 +1956,13 @@
       <c r="T17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="U17" s="2" t="s">
+      <c r="U17" s="17" t="s">
         <v>20</v>
       </c>
       <c r="V17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W17" s="2" t="s">
+      <c r="W17" s="18" t="s">
         <v>20</v>
       </c>
       <c r="X17" s="3">
@@ -1960,7 +2050,7 @@
       <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="14" t="s">
         <v>17</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -2073,7 +2163,7 @@
       <c r="O20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="P20" s="2" t="s">
+      <c r="P20" s="18" t="s">
         <v>20</v>
       </c>
       <c r="Q20" s="2" t="s">
@@ -2200,7 +2290,7 @@
       <c r="H22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="I22" s="17" t="s">
         <v>20</v>
       </c>
       <c r="J22" s="1" t="s">
@@ -2318,6 +2408,42 @@
       </c>
       <c r="W23" s="3">
         <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B25" s="7"/>
+      <c r="C25" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B26" s="8"/>
+      <c r="C26" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B27" s="9"/>
+      <c r="C27" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B28" s="11"/>
+      <c r="C28" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B29" s="12"/>
+      <c r="C29" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B30" s="10"/>
+      <c r="C30" s="13" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished Part II - fixed excel file
</commit_message>
<xml_diff>
--- a/OurClues/ClueLayout_Excel.xlsx
+++ b/OurClues/ClueLayout_Excel.xlsx
@@ -606,7 +606,7 @@
   <dimension ref="A1:AC30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R27" sqref="R27"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,7 +732,7 @@
       <c r="N2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="18" t="s">
         <v>24</v>
       </c>
       <c r="P2" s="1" t="s">

</xml_diff>